<commit_message>
Creation utilisateur sur page inscription marche
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /Livrable1/Livrable2/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /Livrable2/Untitled/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326D6F17-8D1B-D643-AD3F-5BB5475B2207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F55DDE8-FF18-0640-8F5C-42987985AAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
   <si>
     <t>Temps</t>
   </si>
@@ -73,15 +73,6 @@
   </si>
   <si>
     <t>Entrevue avec le client</t>
-  </si>
-  <si>
-    <t>Modifications diagrammes</t>
-  </si>
-  <si>
-    <t>Aide des coéquipiers</t>
-  </si>
-  <si>
-    <t>Travail sur modele de BD</t>
   </si>
   <si>
     <t>Rédaction</t>
@@ -157,6 +148,9 @@
   </si>
   <si>
     <t>t</t>
+  </si>
+  <si>
+    <t>Création de compte BD</t>
   </si>
 </sst>
 </file>
@@ -613,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -646,13 +640,13 @@
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -666,7 +660,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="9">
         <v>5</v>
@@ -675,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E4" s="9">
         <v>0</v>
@@ -686,13 +680,13 @@
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
@@ -706,13 +700,13 @@
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="9">
         <v>0</v>
@@ -734,7 +728,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -746,7 +740,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9">
@@ -758,7 +752,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -770,7 +764,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9">
@@ -792,16 +786,19 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -832,36 +829,23 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="F2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -919,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -933,13 +917,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>2.5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -947,7 +931,7 @@
         <v>1.5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -955,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1011,13 +995,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="12"/>
       <c r="H2" s="12"/>
@@ -1028,13 +1012,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F3" s="12"/>
       <c r="H3" s="12"/>
@@ -1046,7 +1030,7 @@
         <v>0.5</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" s="12"/>
       <c r="H4" s="12"/>
@@ -1058,7 +1042,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F5" s="12"/>
       <c r="H5" s="12"/>
@@ -1070,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="12"/>
       <c r="H6" s="12"/>
@@ -8091,13 +8075,13 @@
         <v>4.5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2">
         <v>4.5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8105,7 +8089,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8113,7 +8097,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -8122,6 +8106,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -8354,24 +8355,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8388,29 +8397,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modidfication document word et excel
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /Livrable2/Untitled/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043607E2-C67E-A84C-BA79-903037749667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2AE757-4904-BD45-96E6-981874C509F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
   <si>
     <t>Temps</t>
   </si>
@@ -73,15 +73,6 @@
   </si>
   <si>
     <t>Entrevue avec le client</t>
-  </si>
-  <si>
-    <t>Modifications diagrammes</t>
-  </si>
-  <si>
-    <t>Aide des coéquipiers</t>
-  </si>
-  <si>
-    <t>Travail sur modele de BD</t>
   </si>
   <si>
     <t>Rédaction</t>
@@ -141,9 +132,6 @@
     <t>4h</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>Corriger Document Analyse</t>
   </si>
   <si>
@@ -157,9 +145,6 @@
   </si>
   <si>
     <t>Création d'utilisateur dans le page d'inscription</t>
-  </si>
-  <si>
-    <t>6 heures</t>
   </si>
 </sst>
 </file>
@@ -619,8 +604,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -652,13 +637,13 @@
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -672,7 +657,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="9">
         <v>5</v>
@@ -684,21 +669,21 @@
         <v>0</v>
       </c>
       <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10">
         <v>6</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
@@ -712,13 +697,13 @@
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="D6" s="9">
         <v>0</v>
@@ -740,7 +725,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6">
@@ -752,7 +737,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9">
@@ -764,7 +749,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6">
@@ -776,7 +761,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9">
@@ -798,18 +783,22 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="2" max="2" width="87.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="58" customWidth="1"/>
+    <col min="10" max="10" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -840,42 +829,31 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="13"/>
       <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>38</v>
+        <v>3</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="F2" s="13"/>
+      <c r="I2" s="13">
+        <v>6</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="2">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -933,7 +911,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -947,13 +925,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>2.5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -961,7 +939,7 @@
         <v>1.5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -969,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1031,10 +1009,10 @@
       <c r="G2" s="14"/>
       <c r="H2" s="12"/>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.15">
@@ -1045,10 +1023,10 @@
       <c r="F3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="13" x14ac:dyDescent="0.15">
@@ -8090,13 +8068,13 @@
         <v>4.5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2">
         <v>4.5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8104,7 +8082,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8112,7 +8090,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -8121,6 +8099,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -8353,38 +8348,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8407,9 +8374,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correction de fautes et ajout de mes heures dans la feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanid\OneDrive\Documents\GitHub\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75431678-341B-4229-982B-E6E36F2EEC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F850A0FF-3C23-48EB-808E-E8A54C281540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
   <si>
     <t>Temps</t>
   </si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>2h30 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 min </t>
+  </si>
+  <si>
+    <t>Modification du document analyse préliminaire</t>
+  </si>
+  <si>
+    <t>8h</t>
   </si>
 </sst>
 </file>
@@ -613,8 +622,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -660,8 +669,8 @@
       <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="7">
-        <v>0</v>
+      <c r="F3" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -962,8 +971,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1055,13 +1064,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
       <c r="F6" s="12"/>
       <c r="H6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
@@ -8109,23 +8123,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -8358,10 +8355,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8384,20 +8409,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Création du diagramme de cas d'utilisation et mise à jour de ma feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanid\OneDrive\Documents\GitHub\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213C17E1-6313-469D-BB6E-6AA22C8E538C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DC4F6C-4310-4975-8E19-5A29FECCE192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>Temps</t>
   </si>
@@ -156,7 +156,10 @@
     <t>Modification du document analyse préliminaire</t>
   </si>
   <si>
-    <t>8h</t>
+    <t>Création du diagramme de cas d'utilisation</t>
+  </si>
+  <si>
+    <t>8h30</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -303,7 +306,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +626,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,7 +673,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
@@ -971,7 +973,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1076,14 +1078,19 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="D7" s="12"/>
       <c r="F7" s="12"/>
       <c r="H7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="D8" s="12"/>
       <c r="F8" s="12"/>
@@ -8123,7 +8130,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I5" s="17">
+      <c r="I5">
         <v>0.5</v>
       </c>
       <c r="J5" t="s">
@@ -8136,12 +8143,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8378,17 +8384,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8413,18 +8429,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Le bouton "Voir le produit" permet à utilisateur de voir  la description de la produit.
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2244482\Documents\GitHub\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B3B000-EE96-44F8-B715-970FBF93A4BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963E8D38-B7F4-44F3-86B2-553D9C4DE906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="7785" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="56">
   <si>
     <t>Temps</t>
   </si>
@@ -197,12 +197,24 @@
   <si>
     <t>chercher le produit quand on click</t>
   </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>modification des imgs</t>
+  </si>
+  <si>
+    <t>Creation d'une page pour la description des produits. (Chercher produit et afficher)</t>
+  </si>
+  <si>
+    <t>6.5h</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -231,6 +243,10 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -668,20 +684,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -700,8 +716,11 @@
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -720,8 +739,9 @@
       <c r="F3" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -740,8 +760,9 @@
       <c r="F4" s="10">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -758,10 +779,11 @@
         <v>18</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -780,8 +802,9 @@
       <c r="F6" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -789,7 +812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -801,7 +824,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -813,7 +836,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -825,7 +848,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -838,6 +861,7 @@
       <c r="F12" s="10"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -847,10 +871,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="B1" zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -862,7 +886,7 @@
     <col min="10" max="10" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -893,8 +917,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -906,7 +936,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="13"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -917,15 +947,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -935,10 +966,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -946,9 +977,10 @@
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="10" max="10" width="23.28515625" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -979,8 +1011,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -997,8 +1035,11 @@
       <c r="J2" s="17" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1016,7 +1057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="G4" s="15" t="s">
@@ -1025,8 +1066,14 @@
       <c r="H4" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="15" t="s">
@@ -1036,9 +1083,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1048,15 +1096,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1087,8 +1135,14 @@
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="12"/>
       <c r="C2" s="2"/>
@@ -1103,7 +1157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1117,7 +1171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
@@ -1130,7 +1184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
@@ -1143,7 +1197,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
@@ -1156,7 +1210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="12"/>
       <c r="D7" s="12"/>
       <c r="F7" s="12"/>
@@ -1168,7 +1222,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>
       <c r="D8" s="12"/>
       <c r="F8" s="12"/>
@@ -1180,7 +1234,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>
       <c r="D9" s="12"/>
       <c r="F9" s="12"/>
@@ -1192,49 +1246,49 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="F10" s="12"/>
       <c r="H10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="12"/>
       <c r="D11" s="12"/>
       <c r="F11" s="12"/>
       <c r="H11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
       <c r="D12" s="12"/>
       <c r="F12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="12"/>
       <c r="D13" s="12"/>
       <c r="F13" s="12"/>
       <c r="H13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="12"/>
       <c r="D14" s="12"/>
       <c r="F14" s="12"/>
       <c r="H14" s="12"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="12"/>
       <c r="D15" s="12"/>
       <c r="F15" s="12"/>
       <c r="H15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="12"/>
       <c r="D16" s="12"/>
       <c r="F16" s="12"/>
@@ -8130,6 +8184,7 @@
       <c r="J1000" s="12"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8139,10 +8194,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8151,9 +8206,10 @@
     <col min="4" max="4" width="32" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -8184,8 +8240,14 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -8197,7 +8259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="I3">
@@ -8207,7 +8269,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="I4">
@@ -8217,7 +8279,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5">
         <v>0.5</v>
       </c>
@@ -8226,17 +8288,17 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8473,17 +8535,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8508,18 +8580,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix du problème de sauvegarde dans la page de paramètre utilisateur et mise à jour de mon suivi et de ma feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF78288-CDB5-884A-8BCF-AF050B9F3B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C1BDA1-9F5B-FE44-906F-19A16B478FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
   <si>
     <t>Temps</t>
   </si>
@@ -197,6 +197,12 @@
   <si>
     <t>Ajouter produit au panier</t>
   </si>
+  <si>
+    <t>2 heures</t>
+  </si>
+  <si>
+    <t>Règler un problème de sauvegarde dans la page paramètre utiliseur</t>
+  </si>
 </sst>
 </file>
 
@@ -302,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -350,6 +356,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -849,7 +858,7 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
+    <sheetView zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1055,15 +1064,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1094,8 +1103,14 @@
       <c r="J1" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+      <c r="K1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="12"/>
       <c r="C2" s="2"/>
@@ -1109,8 +1124,14 @@
       <c r="J2" s="12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+      <c r="K2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="42" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1124,7 +1145,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="28" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" ht="28" x14ac:dyDescent="0.15">
       <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
@@ -1137,7 +1158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.15">
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
@@ -1150,7 +1171,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="56" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" ht="56" x14ac:dyDescent="0.15">
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
@@ -1163,7 +1184,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="12"/>
       <c r="D7" s="12"/>
       <c r="F7" s="12"/>
@@ -1175,7 +1196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12"/>
       <c r="D8" s="12"/>
       <c r="F8" s="12"/>
@@ -1187,7 +1208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12"/>
       <c r="D9" s="12"/>
       <c r="F9" s="12"/>
@@ -1199,49 +1220,49 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="F10" s="12"/>
       <c r="H10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="12"/>
       <c r="D11" s="12"/>
       <c r="F11" s="12"/>
       <c r="H11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="12"/>
       <c r="D12" s="12"/>
       <c r="F12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="12"/>
       <c r="D13" s="12"/>
       <c r="F13" s="12"/>
       <c r="H13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12"/>
       <c r="D14" s="12"/>
       <c r="F14" s="12"/>
       <c r="H14" s="12"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12"/>
       <c r="D15" s="12"/>
       <c r="F15" s="12"/>
       <c r="H15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12"/>
       <c r="D16" s="12"/>
       <c r="F16" s="12"/>
@@ -8238,12 +8259,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8480,17 +8500,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8515,18 +8545,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ajout du nouveau modèle logique et mise à jour du mon suivi et ma feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C1BDA1-9F5B-FE44-906F-19A16B478FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE4B1DA-00EB-104C-9D5A-374C2A661CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
   <si>
     <t>Temps</t>
   </si>
@@ -203,6 +203,21 @@
   <si>
     <t>Règler un problème de sauvegarde dans la page paramètre utiliseur</t>
   </si>
+  <si>
+    <t>Modification du  modèle logique pour ajouter des nouvelles tables</t>
+  </si>
+  <si>
+    <t>5 heures</t>
+  </si>
+  <si>
+    <t>Fonctionnement du ajout produit afin que les produits soient stocké dans la base de donnée</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>6 heures</t>
+  </si>
 </sst>
 </file>
 
@@ -308,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,6 +375,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,20 +693,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -709,8 +725,11 @@
       <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G2" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -729,8 +748,11 @@
       <c r="F3" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G3" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -749,8 +771,9 @@
       <c r="F4" s="10">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -769,8 +792,9 @@
       <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -789,8 +813,9 @@
       <c r="F6" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G6" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -798,7 +823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -810,7 +835,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -822,7 +847,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -834,7 +859,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -858,7 +883,7 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -1067,7 +1092,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1131,7 +1156,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="42" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" ht="56" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1144,8 +1169,14 @@
       <c r="J3" s="12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="28" x14ac:dyDescent="0.15">
+      <c r="K3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="84" x14ac:dyDescent="0.15">
       <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
@@ -1156,6 +1187,12 @@
       </c>
       <c r="J4" s="12" t="s">
         <v>25</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.15">
@@ -1213,19 +1250,18 @@
       <c r="D9" s="12"/>
       <c r="F9" s="12"/>
       <c r="H9" s="12"/>
-      <c r="I9" s="15" t="s">
-        <v>14</v>
+      <c r="I9" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="J9" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="F10" s="12"/>
       <c r="H10" s="12"/>
-      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="12"/>
@@ -8259,11 +8295,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8500,27 +8537,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8545,9 +8572,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mis a jour feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F6C712-3F73-544A-9CD3-72416D83EDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B0E8FC-3F38-D343-9D40-7CA9FB0CFAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="760" windowWidth="26440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="760" windowWidth="26440" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -729,8 +729,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -813,7 +813,9 @@
       <c r="F4" s="26">
         <v>6</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="26">
+        <v>4</v>
+      </c>
       <c r="H4" s="26"/>
       <c r="I4" s="26"/>
     </row>
@@ -932,8 +934,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25:K26"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8432,6 +8434,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -8664,38 +8683,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8718,9 +8709,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise à jour du mon suivi et de ma feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F6C712-3F73-544A-9CD3-72416D83EDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D431F22-D673-ED42-B978-0FC00EACE823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="760" windowWidth="26440" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
   <si>
     <t>Temps</t>
   </si>
@@ -229,6 +229,15 @@
   </si>
   <si>
     <t>8h</t>
+  </si>
+  <si>
+    <t>4 heures</t>
+  </si>
+  <si>
+    <t>Refaire le design de la page paramètre utilisateur au complet</t>
+  </si>
+  <si>
+    <t>Ajouter la fonctionnalité de créer un nouveau mot de passe avec bycrypt pour mettre en hashage tous les mots de passe des utilisateurs en sécurté.</t>
   </si>
 </sst>
 </file>
@@ -730,7 +739,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -813,7 +822,9 @@
       <c r="F4" s="26">
         <v>6</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="26" t="s">
+        <v>19</v>
+      </c>
       <c r="H4" s="26"/>
       <c r="I4" s="26"/>
     </row>
@@ -836,7 +847,9 @@
       <c r="F5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="24"/>
+      <c r="G5" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
     </row>
@@ -859,7 +872,9 @@
       <c r="F6" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="26"/>
+      <c r="G6" s="26" t="s">
+        <v>38</v>
+      </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
     </row>
@@ -1191,8 +1206,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1267,8 +1282,14 @@
       <c r="L2" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="42" x14ac:dyDescent="0.15">
+      <c r="M2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="168" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1286,6 +1307,12 @@
       </c>
       <c r="L3" s="12" t="s">
         <v>59</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="84" x14ac:dyDescent="0.15">
@@ -8432,6 +8459,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -8664,38 +8708,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8718,9 +8734,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
la partie résumée de la page panier, calculer le montant  totale dans le panier et modification du arriere plan
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D431F22-D673-ED42-B978-0FC00EACE823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80A0177-6FF5-1545-9370-8760772E6CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="67">
   <si>
     <t>Temps</t>
   </si>
@@ -239,6 +239,9 @@
   <si>
     <t>Ajouter la fonctionnalité de créer un nouveau mot de passe avec bycrypt pour mettre en hashage tous les mots de passe des utilisateurs en sécurté.</t>
   </si>
+  <si>
+    <t>Faire la partie résumée de la page panier, calculer le montant  totale dans le panier</t>
+  </si>
 </sst>
 </file>
 
@@ -349,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -418,6 +421,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,7 +747,7 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -947,8 +956,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="108" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25:K26"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -959,6 +968,7 @@
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="37.33203125" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="14" max="14" width="59.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1011,7 +1021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="13"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1028,8 +1038,15 @@
       <c r="L2" s="13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M2" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="O2" s="28"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="13"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1039,6 +1056,8 @@
       <c r="J3" s="13" t="s">
         <v>48</v>
       </c>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="2"/>
@@ -1207,7 +1226,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8459,23 +8478,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -8708,10 +8710,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8734,20 +8764,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
mise a jour de ma feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000BB51D-9D64-CD47-B546-6EA6E4B19D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BD473F-EDE4-2C4F-A553-CC8382FD54BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -8517,12 +8517,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8759,17 +8758,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8794,18 +8803,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
La page paiement front end et back end et modification du server.js
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38467CAC-D542-A646-8E37-67B88DA27E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C5F381-F5D1-D44E-B982-9F75FFF8BD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="760" windowWidth="26440" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="77">
   <si>
     <t>Temps</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>ajustement du code js server pour permettre l'affichage des données utilisateur dans la page paramètre</t>
+  </si>
+  <si>
+    <t>Faire la page de transaction (Front-end et Back-end</t>
   </si>
 </sst>
 </file>
@@ -775,7 +778,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -866,7 +869,9 @@
       <c r="H4" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="26"/>
+      <c r="I4" s="26" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -993,8 +998,8 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="L1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1006,6 +1011,7 @@
     <col min="10" max="10" width="37.33203125" customWidth="1"/>
     <col min="12" max="12" width="21" customWidth="1"/>
     <col min="14" max="14" width="59.33203125" customWidth="1"/>
+    <col min="16" max="16" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
@@ -1081,7 +1087,12 @@
       <c r="N2" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="O2" s="28"/>
+      <c r="O2" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="13"/>
@@ -8561,11 +8572,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8802,27 +8814,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8847,9 +8849,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise a jour de ma feuille de temps et suivi
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C5F381-F5D1-D44E-B982-9F75FFF8BD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDED81E-AC5B-C145-AD9E-1DD51901DC1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="760" windowWidth="26440" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
   <si>
     <t>Temps</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Faire la page de transaction (Front-end et Back-end</t>
+  </si>
+  <si>
+    <t>6 heures</t>
+  </si>
+  <si>
+    <t>Implémentation du NoSQL dans le projet en replaçant la table utilisateur avec la collection "utilisateurs"</t>
   </si>
 </sst>
 </file>
@@ -777,8 +783,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -842,7 +848,9 @@
       <c r="H3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="24"/>
+      <c r="I3" s="24" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -998,7 +1006,7 @@
   </sheetPr>
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -1293,8 +1301,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1349,7 +1357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="84" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="98" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="12"/>
       <c r="C2" s="2"/>
@@ -1374,6 +1382,12 @@
       </c>
       <c r="N2" s="18" t="s">
         <v>64</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="168" x14ac:dyDescent="0.15">
@@ -8433,8 +8447,8 @@
   </sheetPr>
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8497,7 +8511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="41.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -8505,52 +8519,51 @@
       <c r="I2" s="15">
         <v>0.5</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="20"/>
+      <c r="K2" s="15">
+        <v>2</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="M2" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" s="15">
-        <v>1</v>
-      </c>
-      <c r="P2" s="20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="46.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="97" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="I3" s="15">
         <v>0.5</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="16">
+      <c r="K3" s="16">
         <v>2</v>
       </c>
+      <c r="L3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="15">
+        <v>1</v>
+      </c>
       <c r="N3" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="O3" s="15">
-        <v>1</v>
-      </c>
-      <c r="P3" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="I4" s="15">
         <v>3</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="J4" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -8558,7 +8571,7 @@
       <c r="I5" s="15">
         <v>0.5</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="20" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Travail sur l'API de envoie de courriel et connexion apres inscription
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2244482\Documents\GitHub\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Application Web\tp\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B8E6F3-E59A-4448-964D-7DFAC864D713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D10D95C-07D0-4E45-A6A6-EC8FF0969CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1935" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13725" yWindow="3960" windowWidth="23085" windowHeight="15420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="88">
   <si>
     <t>Temps</t>
   </si>
@@ -286,6 +286,24 @@
   </si>
   <si>
     <t>3.5h</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>creation de footer</t>
+  </si>
+  <si>
+    <t>Connexion d'utilisateurs apres l'inscription</t>
+  </si>
+  <si>
+    <t>Envoie d'une courriel de reinitialisation de mot de passe</t>
+  </si>
+  <si>
+    <t>11h</t>
   </si>
 </sst>
 </file>
@@ -802,20 +820,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -843,8 +861,11 @@
       <c r="I2" s="22" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J2" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -872,8 +893,9 @@
       <c r="I3" s="24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -901,8 +923,9 @@
       <c r="I4" s="26" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -930,8 +953,11 @@
       <c r="I5" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="J5" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -959,8 +985,9 @@
       <c r="I6" s="26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="26"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -968,7 +995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -980,7 +1007,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -992,7 +1019,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1004,7 +1031,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1157,10 +1184,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1172,9 +1199,10 @@
     <col min="12" max="12" width="20.7109375" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="16" max="16" width="21.28515625" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1223,8 +1251,20 @@
       <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1259,8 +1299,14 @@
       <c r="P2" s="29" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1295,8 +1341,14 @@
       <c r="P3" s="29" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="G4" s="15" t="s">
@@ -1311,8 +1363,14 @@
       <c r="J4" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="15" t="s">
@@ -1322,8 +1380,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:20" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Réussir à faire fonctionner la page paramètre avec la collection utilisateurs NoSQL et mise à jour de ma feuille de temps et suivi et modification du script
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E8D612-6FA3-964F-BDF5-BD6E2F242D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31846863-71D8-2942-A58B-B6B83869EEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="93">
   <si>
     <t>Temps</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>9h</t>
+  </si>
+  <si>
+    <t>Réussi à faire fonctionner la collection utilisateurs avec les tables detail_panier et panier pour l'affichage des produits pour chaque utilisateur</t>
   </si>
 </sst>
 </file>
@@ -832,20 +835,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -876,8 +879,11 @@
       <c r="J2" s="22" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="K2" s="22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -908,8 +914,9 @@
       <c r="J3" s="24" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="K3" s="24"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -940,8 +947,9 @@
       <c r="J4" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -972,8 +980,9 @@
       <c r="J5" s="24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="K5" s="24"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1002,8 +1011,9 @@
         <v>27</v>
       </c>
       <c r="J6" s="26"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="26"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1011,7 +1021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1023,7 +1033,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1035,7 +1045,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1047,7 +1057,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1082,7 @@
   </sheetPr>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+    <sheetView zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
       <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
@@ -1424,15 +1434,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R1000"/>
+  <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1487,8 +1497,14 @@
       <c r="R1" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="112" x14ac:dyDescent="0.15">
+      <c r="S1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="154" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="12"/>
       <c r="C2" s="2"/>
@@ -1526,8 +1542,14 @@
       <c r="R2" s="18" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="168" x14ac:dyDescent="0.15">
+      <c r="S2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="168" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1553,7 +1575,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="84" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:20" ht="84" x14ac:dyDescent="0.15">
       <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
@@ -1572,7 +1594,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" ht="42" x14ac:dyDescent="0.15">
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
@@ -1585,7 +1607,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="56" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" ht="56" x14ac:dyDescent="0.15">
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
@@ -1598,7 +1620,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="12"/>
       <c r="D7" s="12"/>
       <c r="F7" s="12"/>
@@ -1610,7 +1632,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12"/>
       <c r="D8" s="12"/>
       <c r="F8" s="12"/>
@@ -1622,7 +1644,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12"/>
       <c r="D9" s="12"/>
       <c r="F9" s="12"/>
@@ -1634,49 +1656,49 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="F10" s="12"/>
       <c r="H10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="12"/>
       <c r="D11" s="12"/>
       <c r="F11" s="12"/>
       <c r="H11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="12"/>
       <c r="D12" s="12"/>
       <c r="F12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="12"/>
       <c r="D13" s="12"/>
       <c r="F13" s="12"/>
       <c r="H13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12"/>
       <c r="D14" s="12"/>
       <c r="F14" s="12"/>
       <c r="H14" s="12"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12"/>
       <c r="D15" s="12"/>
       <c r="F15" s="12"/>
       <c r="H15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12"/>
       <c r="D16" s="12"/>
       <c r="F16" s="12"/>
@@ -8722,11 +8744,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8963,27 +8986,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9008,9 +9021,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modification du page Affichage page paiement (saisie automatique)
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31846863-71D8-2942-A58B-B6B83869EEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0DBA23-1842-D749-8A51-05107DB95B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="95">
   <si>
     <t>Temps</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>Réussi à faire fonctionner la collection utilisateurs avec les tables detail_panier et panier pour l'affichage des produits pour chaque utilisateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification du page Affichage </t>
+  </si>
+  <si>
+    <t>page paiement (saisie automatique)</t>
   </si>
 </sst>
 </file>
@@ -837,8 +843,8 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -947,7 +953,9 @@
       <c r="J4" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="26"/>
+      <c r="K4" s="26" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1080,10 +1088,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="P1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1097,10 +1105,11 @@
     <col min="14" max="14" width="59.33203125" customWidth="1"/>
     <col min="16" max="16" width="50.83203125" customWidth="1"/>
     <col min="17" max="17" width="20.6640625" customWidth="1"/>
-    <col min="18" max="18" width="47.33203125" customWidth="1"/>
+    <col min="18" max="18" width="55.5" customWidth="1"/>
+    <col min="20" max="20" width="56.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1155,8 +1164,14 @@
       <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="13"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1191,8 +1206,14 @@
       <c r="R2" s="13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="13"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1204,12 +1225,18 @@
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="28"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="S3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
@@ -8753,6 +8780,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -8985,14 +9020,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
@@ -9002,6 +9029,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9018,21 +9062,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fin de  travail sur l'API de reinitialisation de mot de passe
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2244482\Documents\GitHub\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Application Web\tp\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CFF234-33D6-4D9B-8C44-8875093B4062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C0F696-5121-4DE7-BCED-BA5C201CB065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30075" yWindow="5115" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="3810" windowWidth="23085" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="98">
   <si>
     <t>Temps</t>
   </si>
@@ -322,6 +322,18 @@
   </si>
   <si>
     <t>Validation de mot de passe</t>
+  </si>
+  <si>
+    <t>Envoie de courriel fin d'API</t>
+  </si>
+  <si>
+    <t>Cherche des produit en cliquant sur lees images</t>
+  </si>
+  <si>
+    <t>.5h</t>
+  </si>
+  <si>
+    <t>interface pour le reinitialisation de mot de passe</t>
   </si>
 </sst>
 </file>
@@ -439,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -520,6 +532,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,8 +855,8 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -983,7 +998,9 @@
       <c r="J5" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K5" s="24"/>
+      <c r="K5" s="24" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -1229,8 +1246,8 @@
   </sheetPr>
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1243,6 +1260,7 @@
     <col min="14" max="14" width="19" customWidth="1"/>
     <col min="16" max="16" width="21.28515625" customWidth="1"/>
     <col min="18" max="18" width="19.140625" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" x14ac:dyDescent="0.25">
@@ -1396,8 +1414,14 @@
       <c r="R3" s="16" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="G4" s="15" t="s">
@@ -1418,8 +1442,14 @@
       <c r="R4" s="16" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S4" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="G5" s="15" t="s">
@@ -1427,6 +1457,12 @@
       </c>
       <c r="H5" s="16" t="s">
         <v>44</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="T5" s="31" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8762,14 +8798,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -9002,6 +9030,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
@@ -9011,23 +9047,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9044,4 +9063,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Travail sur le test de detail produit et inscription
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Application Web\tp\TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D08A5E-1F81-4979-8661-7E089AFACAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B868A503-1A25-4731-881F-B0E57D6C7A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="4920" windowWidth="23085" windowHeight="15420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="1860" windowWidth="23085" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="117">
   <si>
     <t>Temps</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>Fin de changement de mot de passe avec l'API</t>
+  </si>
+  <si>
+    <t>Changement de test de l'inscription et travail sur le test de detail produit</t>
   </si>
 </sst>
 </file>
@@ -904,20 +907,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -954,8 +957,11 @@
       <c r="L2" s="22" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="M2" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -992,8 +998,9 @@
       <c r="L3" s="24" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="M3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -1030,8 +1037,9 @@
       <c r="L4" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="M4" s="26"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1068,8 +1076,9 @@
       <c r="L5" s="24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="M5" s="24"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1102,8 +1111,9 @@
         <v>62</v>
       </c>
       <c r="L6" s="26"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="26"/>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1111,7 +1121,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1123,7 +1133,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1135,7 +1145,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1147,7 +1157,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1348,8 +1358,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1363,6 +1373,7 @@
     <col min="16" max="16" width="21.28515625" customWidth="1"/>
     <col min="18" max="18" width="19.140625" customWidth="1"/>
     <col min="20" max="20" width="21.42578125" customWidth="1"/>
+    <col min="24" max="24" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.25">
@@ -1553,13 +1564,13 @@
         <v>108</v>
       </c>
       <c r="W3" s="15" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="X3" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="G4" s="15" t="s">
@@ -1591,6 +1602,12 @@
       </c>
       <c r="V4" s="16" t="s">
         <v>109</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="X4" s="16" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8992,15 +9009,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -9233,6 +9241,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
   <ds:schemaRefs>
@@ -9251,14 +9268,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9275,4 +9284,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mis a jour document word et excel
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84653E6B-8325-A745-874C-1DFFD1D747A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29EF9BA-3E45-154E-9F15-829E8F443BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -921,8 +921,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1193,8 +1193,8 @@
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView topLeftCell="T1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Insertion de la page paiement succès et mise à jour de mon suivi
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD67B99-579E-9E49-91E5-33EF196B1F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB433D40-7AEF-0246-A75B-7F48A1279901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="123">
   <si>
     <t>Temps</t>
   </si>
@@ -394,6 +394,21 @@
   </si>
   <si>
     <t>modification page inscription, mdp oublie, page connexion et reset et l'index</t>
+  </si>
+  <si>
+    <t>Modification de l'interface de la page Paiement</t>
+  </si>
+  <si>
+    <t>Modification de l'interface de la page Paiement Succès</t>
+  </si>
+  <si>
+    <t>Fix des bugs dans la page inscription</t>
+  </si>
+  <si>
+    <t>Affichage des informations dans la page paramètre dans les placeholders</t>
+  </si>
+  <si>
+    <t>9h30</t>
   </si>
 </sst>
 </file>
@@ -520,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -602,8 +617,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,8 +943,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1013,6 +1032,9 @@
       <c r="L3" s="24" t="s">
         <v>42</v>
       </c>
+      <c r="M3" s="24" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -1052,7 +1074,7 @@
         <v>62</v>
       </c>
       <c r="M4" s="31" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -1091,6 +1113,9 @@
       </c>
       <c r="L5" s="24" t="s">
         <v>15</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
@@ -1196,8 +1221,8 @@
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1214,6 +1239,7 @@
     <col min="18" max="18" width="55.5" customWidth="1"/>
     <col min="20" max="20" width="56.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="71.33203125" customWidth="1"/>
+    <col min="24" max="24" width="57.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.2">
@@ -1384,7 +1410,7 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
@@ -1659,15 +1685,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V1000"/>
+  <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1734,8 +1760,14 @@
       <c r="V1" s="11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="154" x14ac:dyDescent="0.15">
+      <c r="W1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="154" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="12"/>
       <c r="C2" s="2"/>
@@ -1785,8 +1817,14 @@
       <c r="V2" s="18" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="168" x14ac:dyDescent="0.15">
+      <c r="W2" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="168" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
@@ -1823,8 +1861,14 @@
       <c r="V3" s="18" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="98" x14ac:dyDescent="0.15">
+      <c r="W3" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="X3" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="98" x14ac:dyDescent="0.15">
       <c r="B4" s="12"/>
       <c r="C4" s="2"/>
       <c r="D4" s="12"/>
@@ -1848,8 +1892,14 @@
       <c r="T4" s="18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="42" x14ac:dyDescent="0.15">
+      <c r="W4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="70" x14ac:dyDescent="0.15">
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="12"/>
@@ -1861,8 +1911,14 @@
       <c r="J5" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="56" x14ac:dyDescent="0.15">
+      <c r="W5" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="X5" s="33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="56" x14ac:dyDescent="0.15">
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
@@ -1875,7 +1931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="12"/>
       <c r="D7" s="12"/>
       <c r="F7" s="12"/>
@@ -1887,7 +1943,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="34.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="12"/>
       <c r="D8" s="12"/>
       <c r="F8" s="12"/>
@@ -1899,7 +1955,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="12"/>
       <c r="D9" s="12"/>
       <c r="F9" s="12"/>
@@ -1911,49 +1967,49 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="F10" s="12"/>
       <c r="H10" s="12"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="12"/>
       <c r="D11" s="12"/>
       <c r="F11" s="12"/>
       <c r="H11" s="12"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="12"/>
       <c r="D12" s="12"/>
       <c r="F12" s="12"/>
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="12"/>
       <c r="D13" s="12"/>
       <c r="F13" s="12"/>
       <c r="H13" s="12"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="12"/>
       <c r="D14" s="12"/>
       <c r="F14" s="12"/>
       <c r="H14" s="12"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="12"/>
       <c r="D15" s="12"/>
       <c r="F15" s="12"/>
       <c r="H15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="12"/>
       <c r="D16" s="12"/>
       <c r="F16" s="12"/>
@@ -9020,6 +9076,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -9252,24 +9325,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9286,29 +9367,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFC7423F-A5DF-42C5-A87D-48923333384C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Réussi à faire sauvegarder dans la base de donnée les commandes
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A5A1B1-F057-D74E-BF14-6D2A4F6E2630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC2B658-6FC6-7A41-AE8E-0C388C820122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
   <si>
     <t>Temps</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>Affichage des informations dans la page paramètre dans les placeholders</t>
+  </si>
+  <si>
+    <t>Réussi à sauvegarder les commandes des utilisateurs dans la base de données</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -610,6 +613,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1209,7 +1216,7 @@
   </sheetPr>
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+    <sheetView topLeftCell="U1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
@@ -1681,8 +1688,8 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView tabSelected="1" topLeftCell="O2" zoomScale="107" workbookViewId="0">
+      <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1912,7 +1919,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="56" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="84" x14ac:dyDescent="0.15">
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
       <c r="D6" s="12"/>
@@ -1923,6 +1930,12 @@
       </c>
       <c r="J6" s="12" t="s">
         <v>37</v>
+      </c>
+      <c r="W6" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="X6" s="32" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="39" customHeight="1" x14ac:dyDescent="0.15">
@@ -9070,6 +9083,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -9302,38 +9332,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9356,9 +9358,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mis a jour documents word et excel
</commit_message>
<xml_diff>
--- a/Documents/Feuille_de_temps_TP.xlsx
+++ b/Documents/Feuille_de_temps_TP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ridhadosh/Documents/GitHub/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanushan/Desktop/Session 4/Application Web /TP_Livrable/TP_Web_Projet_de_Site-Ridha-Thanushan-Dave-Earaj/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC2B658-6FC6-7A41-AE8E-0C388C820122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F06AFE-F0EB-EF46-8292-48C69AAAFBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="127">
   <si>
     <t>Temps</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>Réussi à sauvegarder les commandes des utilisateurs dans la base de données</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>Creation de la page mise A jour Password Success et travailler sur le powerpoint</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -528,11 +534,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB1A0C7"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -614,9 +629,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -935,20 +949,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -988,8 +1002,11 @@
       <c r="M2" s="22" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="N2" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1030,7 +1047,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -1070,8 +1087,11 @@
       <c r="M4" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="N4" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1132,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1167,7 @@
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -1155,7 +1175,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1167,7 +1187,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1179,7 +1199,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1191,7 +1211,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>13</v>
       </c>
@@ -1214,10 +1234,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView topLeftCell="V1" zoomScale="134" zoomScaleNormal="394" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1234,9 +1254,11 @@
     <col min="18" max="18" width="55.5" customWidth="1"/>
     <col min="20" max="20" width="56.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="71.33203125" customWidth="1"/>
+    <col min="24" max="24" width="56.83203125" customWidth="1"/>
+    <col min="26" max="26" width="67" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1309,8 +1331,14 @@
       <c r="X1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="23" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="13"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1363,8 +1391,14 @@
       <c r="X2" s="13" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Y2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="13"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1383,11 +1417,11 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
@@ -1688,7 +1722,7 @@
   </sheetPr>
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O2" zoomScale="107" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="92" workbookViewId="0">
       <selection activeCell="X6" sqref="X6"/>
     </sheetView>
   </sheetViews>
@@ -1931,10 +1965,10 @@
       <c r="J6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="W6" s="31" t="s">
+      <c r="W6" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="X6" s="32" t="s">
+      <c r="X6" s="18" t="s">
         <v>124</v>
       </c>
     </row>
@@ -8924,7 +8958,7 @@
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="R1" sqref="R1:S1"/>
     </sheetView>
   </sheetViews>
@@ -9083,23 +9117,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100106F11FA0920D348AB7B8280E4900B8B" ma:contentTypeVersion="15" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c2e08935190ed95787389072801c2e99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42d21025-700e-4026-9820-3d5a1c2d48f0" xmlns:ns4="5d4e22b2-f71c-440d-92ce-12b46af42ab4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a96be81092f887ae26a0df0d4a7eaeb5" ns3:_="" ns4:_="">
     <xsd:import namespace="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
@@ -9332,10 +9349,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5d4e22b2-f71c-440d-92ce-12b46af42ab4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
+    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9358,20 +9403,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{592B6840-3745-4711-BA23-81EE58995301}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7D2A072-77BD-4ABC-A904-E06B5179D727}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="42d21025-700e-4026-9820-3d5a1c2d48f0"/>
-    <ds:schemaRef ds:uri="5d4e22b2-f71c-440d-92ce-12b46af42ab4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>